<commit_message>
List of parts to print
</commit_message>
<xml_diff>
--- a/Parts to Print.xlsx
+++ b/Parts to Print.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rigorini\Documents\Diego\Progetti Hardware\3DWall\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{44DBF865-3967-4BBD-A14D-1FE240E62DD3}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{BA501CFA-35C9-4025-95BE-AEA72D8B163E}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19560" windowHeight="9525" xr2:uid="{AD4B5A2A-0E8B-44A7-91E1-D202EB516C4D}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="34">
   <si>
     <t>Part number</t>
   </si>
@@ -124,6 +124,9 @@
   </si>
   <si>
     <t>Part 028</t>
+  </si>
+  <si>
+    <t>Part 029</t>
   </si>
 </sst>
 </file>
@@ -186,8 +189,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3F0B421D-98AD-4C35-83D5-D74C9FDB2275}" name="Tabella1" displayName="Tabella1" ref="A1:C29" totalsRowShown="0">
-  <autoFilter ref="A1:C29" xr:uid="{C811CBD2-482C-477C-9EF4-B667A8F59DF2}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3F0B421D-98AD-4C35-83D5-D74C9FDB2275}" name="Tabella1" displayName="Tabella1" ref="A1:C30" totalsRowShown="0">
+  <autoFilter ref="A1:C30" xr:uid="{C811CBD2-482C-477C-9EF4-B667A8F59DF2}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -498,10 +501,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32797C51-70DD-4CCD-9DA5-A660F21D8FD8}">
-  <dimension ref="A1:C29"/>
+  <dimension ref="A1:C30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -830,6 +833,17 @@
         <v>31</v>
       </c>
     </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>33</v>
+      </c>
+      <c r="B30" s="1">
+        <v>1</v>
+      </c>
+      <c r="C30" t="s">
+        <v>31</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>